<commit_message>
handling geopy exceptions and richer output
</commit_message>
<xml_diff>
--- a/data/raw_data/ParisBeerWeek_participants.xlsx
+++ b/data/raw_data/ParisBeerWeek_participants.xlsx
@@ -15,77 +15,14 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$AC$27</definedName>
-    <definedName name="NOM" comment="nom du lieu">Feuil1!$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$AC$30</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Julien Moura</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Julien Moura:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-identifiant incrémental</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Julien Moura:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Soit :
-BAR
-CAVE
-BRASSERIE
-DISTRIBUTEUR</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="404">
   <si>
     <t>ID</t>
   </si>
@@ -129,7 +66,7 @@
     <t>ADR_CONCAT</t>
   </si>
   <si>
-    <t>OSM</t>
+    <t>TEL</t>
   </si>
   <si>
     <t>OSM_URL</t>
@@ -201,6 +138,9 @@
     <t>FRANCE</t>
   </si>
   <si>
+    <t>09 81 12 53 06</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/3512343285</t>
   </si>
   <si>
@@ -225,7 +165,13 @@
     <t>https://plus.google.com/108391973229733464785/about</t>
   </si>
   <si>
-    <t>http://laparisbeerweek.com/2015/wp-content/uploads/2015/03/demory-paris.jpg</t>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/demory-paris.png</t>
+  </si>
+  <si>
+    <t>48.861645</t>
+  </si>
+  <si>
+    <t>2.350797</t>
   </si>
   <si>
     <t>L'Express de Lyon</t>
@@ -243,12 +189,33 @@
     <t>de Lyon</t>
   </si>
   <si>
+    <t>01 43 43 21 32</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/532031656</t>
   </si>
   <si>
     <t>http://laparisbeerweek.com/2015/programme/participant/l-express-de-lyon/</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/l-express-de-lyon-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/lexpress.delyon</t>
+  </si>
+  <si>
+    <t>https://twitter.com/Exss2Lyon</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/lexpress-de-lyon.png</t>
+  </si>
+  <si>
+    <t>48.845825</t>
+  </si>
+  <si>
+    <t>2.372362</t>
+  </si>
+  <si>
     <t>La Fine Mousse</t>
   </si>
   <si>
@@ -270,12 +237,33 @@
     <t>Jean Aicard</t>
   </si>
   <si>
+    <t>09 80 45 94 64</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/1830661957</t>
   </si>
   <si>
     <t>http://laparisbeerweek.com/2015/programme/participant/la-fine-mousse/</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/la-fine-mousse-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/lafinemousse</t>
+  </si>
+  <si>
+    <t>https://twitter.com/lafinemousse</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/la-fine-mousse.png</t>
+  </si>
+  <si>
+    <t>48.864845</t>
+  </si>
+  <si>
+    <t>2.381682</t>
+  </si>
+  <si>
     <t>Le Festin Nu</t>
   </si>
   <si>
@@ -297,6 +285,24 @@
     <t>http://laparisbeerweek.com/2015/programme/participant/le-festin-nu/</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/le-festin-nu-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/LeFestinNu</t>
+  </si>
+  <si>
+    <t>https://twitter.com/FestinNu</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/le-festin-nu.png</t>
+  </si>
+  <si>
+    <t>48.890457</t>
+  </si>
+  <si>
+    <t>2.339149</t>
+  </si>
+  <si>
     <t>Le Supercoin</t>
   </si>
   <si>
@@ -312,12 +318,33 @@
     <t>Baudelique</t>
   </si>
   <si>
+    <t>09 50 07 04 90</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/3434564233</t>
   </si>
   <si>
     <t>http://laparisbeerweek.com/2015/programme/participant/le-supercoin/</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/le-supercoin-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/supercoin</t>
+  </si>
+  <si>
+    <t>https://twitter.com/le_supercoin</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/le-supercoin.png</t>
+  </si>
+  <si>
+    <t>48.892212</t>
+  </si>
+  <si>
+    <t>2.347057</t>
+  </si>
+  <si>
     <t>Les Trois 8</t>
   </si>
   <si>
@@ -333,13 +360,34 @@
     <t>Victor Letalle</t>
   </si>
   <si>
+    <t>01 40 33 47 70</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/2901434882</t>
   </si>
   <si>
     <t>http://laparisbeerweek.com/2015/programme/participant/les-trois-8/</t>
   </si>
   <si>
-    <t>A la bière comme à la bière</t>
+    <t>http://laparisbeerweek.com/2015/programme/participant/les-trois-8-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/lestrois8</t>
+  </si>
+  <si>
+    <t>https://twitter.com/lestrois8</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/les-trois-8.png</t>
+  </si>
+  <si>
+    <t>48.867462</t>
+  </si>
+  <si>
+    <t>2.385138</t>
+  </si>
+  <si>
+    <t>A la bière comme à la bière Jourdain</t>
   </si>
   <si>
     <t>CAVE</t>
@@ -357,10 +405,46 @@
     <t>des Pyrénées</t>
   </si>
   <si>
+    <t>https://www.openstreetmap.org/node/3512354722</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/a-la-biere-comme-a-la-biere/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/a-la-biere-comme-a-la-biere-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/ALaBiereCommeALaBiere</t>
+  </si>
+  <si>
+    <t>https://twitter.com/alabiere</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/a-la-biere-comme-a-la-biere.png</t>
+  </si>
+  <si>
+    <t>48.872513</t>
+  </si>
+  <si>
+    <t>2.39116</t>
+  </si>
+  <si>
+    <t>A la bière comme à la bière Custine</t>
+  </si>
+  <si>
+    <t>Custine</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/3515582589</t>
   </si>
   <si>
-    <t>Bières cultes</t>
+    <t>48.888466</t>
+  </si>
+  <si>
+    <t>2.347723</t>
+  </si>
+  <si>
+    <t>Bières Cultes Cardinal</t>
   </si>
   <si>
     <t>Bières Cultes, c’est quatre caves à bières à Paris, accessibles en métro et en bus, et une sélection des meilleures bières du monde. Bières Cultes propose plusieurs centaines de références ainsi qu’un large choix de produits dérivés : verres, plaques, t-shirts, sous-bocks, etc. Un espace de dégustation accueille également les amateurs dans le magasin de Cardinal-Lemoine (5e arrd.).</t>
@@ -378,6 +462,81 @@
     <t>https://www.openstreetmap.org/node/677805360</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/bieres-cultes/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/bieres-cultes-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/bierescultes</t>
+  </si>
+  <si>
+    <t>https://twitter.com/Bieres_Cultes</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/bieres-cultes.png</t>
+  </si>
+  <si>
+    <t>48.846363</t>
+  </si>
+  <si>
+    <t>2.351918</t>
+  </si>
+  <si>
+    <t>Bières Cultes Damrémont</t>
+  </si>
+  <si>
+    <t>Damrémont</t>
+  </si>
+  <si>
+    <t>40, rue Damrémont, 75018 Paris, FRANCE</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/1916353716#map=19/48.88955/2.33380</t>
+  </si>
+  <si>
+    <t>48.889412</t>
+  </si>
+  <si>
+    <t>2.333632</t>
+  </si>
+  <si>
+    <t>Bières Cultes Legendre</t>
+  </si>
+  <si>
+    <t>Legendre</t>
+  </si>
+  <si>
+    <t>25, rue Legendre, 75017 Paris, FRANCE</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/2876149573</t>
+  </si>
+  <si>
+    <t>48.884155</t>
+  </si>
+  <si>
+    <t>2.314215</t>
+  </si>
+  <si>
+    <t>Bières Cultes Châtelet</t>
+  </si>
+  <si>
+    <t>des Halles</t>
+  </si>
+  <si>
+    <t>14 rue des Halles 75001 Paris</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/677805360#map=19/48.85986/2.34681</t>
+  </si>
+  <si>
+    <t>48.859764</t>
+  </si>
+  <si>
+    <t>2.34669</t>
+  </si>
+  <si>
     <t>Bierissime</t>
   </si>
   <si>
@@ -396,9 +555,30 @@
     <t>de Magenta</t>
   </si>
   <si>
+    <t>01 44 79 02 97</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/3512366899</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/bierissime/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/bierissime-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/Bierissime</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/bierissime.png</t>
+  </si>
+  <si>
+    <t>48.876308</t>
+  </si>
+  <si>
+    <t>2.356019</t>
+  </si>
+  <si>
     <t>Biérocratie</t>
   </si>
   <si>
@@ -414,9 +594,33 @@
     <t>de l'Espérance</t>
   </si>
   <si>
+    <t>01 53 80 16 10</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/2206967422</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/bierocratie/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/bierocratie-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/bierocratie</t>
+  </si>
+  <si>
+    <t>https://twitter.com/bierocratie</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/bierocratie.png</t>
+  </si>
+  <si>
+    <t>48.825516</t>
+  </si>
+  <si>
+    <t>2.34708</t>
+  </si>
+  <si>
     <t>Brewberry</t>
   </si>
   <si>
@@ -432,9 +636,30 @@
     <t>du Pot-de-Fer</t>
   </si>
   <si>
+    <t>01 43 36 53 92</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/1884433764</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/brewberry/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/brewberry-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/pages/BREWBERRY/112193145482420</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/brewberry.png</t>
+  </si>
+  <si>
+    <t>48.842915</t>
+  </si>
+  <si>
+    <t>2.348499</t>
+  </si>
+  <si>
     <t>Chop'in</t>
   </si>
   <si>
@@ -450,9 +675,33 @@
     <t>de Gergovie</t>
   </si>
   <si>
+    <t>01 45 42 93 71</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/2320940893</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/chop-in/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/chop-in-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/pages/CHOP-IN/238925751636</t>
+  </si>
+  <si>
+    <t>https://twitter.com/ChopinMickey</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/chop-in.png</t>
+  </si>
+  <si>
+    <t>48.832993</t>
+  </si>
+  <si>
+    <t>2.316165</t>
+  </si>
+  <si>
     <t>La Cave à Bulles</t>
   </si>
   <si>
@@ -465,9 +714,30 @@
     <t>http://caveabulles.fr/</t>
   </si>
   <si>
+    <t>01 40 29 03 69</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/3458097215</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/la-cave-a-bulles/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/la-cave-a-bulles-en/</t>
+  </si>
+  <si>
+    <t>https://fr-fr.facebook.com/LaCaveaBulles</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/la-cave-a-bulles.png</t>
+  </si>
+  <si>
+    <t>48.861</t>
+  </si>
+  <si>
+    <t>2.350491</t>
+  </si>
+  <si>
     <t>Brasserie de Marcoussis</t>
   </si>
   <si>
@@ -492,9 +762,30 @@
     <t>Marcoussis</t>
   </si>
   <si>
+    <t>09 62 35 27 83</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/way/146093848</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/brasserie-de-marcoussis/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/brasserie-de-marcoussis-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/BrasserieArtisanaleDeMarcoussis</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/brasserie-artisanale-de-marcoussis.png</t>
+  </si>
+  <si>
+    <t>48.660234</t>
+  </si>
+  <si>
+    <t>2.206272</t>
+  </si>
+  <si>
     <t>Brasserie de la Goutte d'or</t>
   </si>
   <si>
@@ -510,9 +801,33 @@
     <t>de la Goutte d'Or</t>
   </si>
   <si>
+    <t>09 80 64 23 51</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/2461799896</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/brasserie-de-la-goutte-dor/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/brasserie-de-la-goutte-dor-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/brasserielagouttedor</t>
+  </si>
+  <si>
+    <t>https://twitter.com/LBGOPARIS</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/brasserie-de-la-goutte-dor.png</t>
+  </si>
+  <si>
+    <t>48.884991</t>
+  </si>
+  <si>
+    <t>2.352359</t>
+  </si>
+  <si>
     <t>Brasserie de la Vallée de Chevreuse</t>
   </si>
   <si>
@@ -534,6 +849,21 @@
     <t>https://www.openstreetmap.org/way/344329214</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/brasserie-de-la-vallee-de-chevreuse/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/brasserie-de-la-vallee-de-chevreuse-en/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/brasserie-de-la-vallee-de-chevreuse.png</t>
+  </si>
+  <si>
+    <t>48.613838</t>
+  </si>
+  <si>
+    <t>2.024662</t>
+  </si>
+  <si>
     <t>Crazy Hops</t>
   </si>
   <si>
@@ -558,6 +888,24 @@
     <t>https://www.openstreetmap.org/node/3515448663</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/crazy-hops/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/crazy-hops-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/bieredelourcq</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/crazy-hops.png</t>
+  </si>
+  <si>
+    <t>48.209836</t>
+  </si>
+  <si>
+    <t>2.971787</t>
+  </si>
+  <si>
     <t>Deck &amp; Donohue</t>
   </si>
   <si>
@@ -576,9 +924,33 @@
     <t>Montreuil</t>
   </si>
   <si>
+    <t>01 60 46 62 33</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/3512392272</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/deck-donohue/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/deck-donohue-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/deckdonohue</t>
+  </si>
+  <si>
+    <t>https://twitter.com/DeckDonohue</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/deck-donohue.png</t>
+  </si>
+  <si>
+    <t>48.858562</t>
+  </si>
+  <si>
+    <t>2.423444</t>
+  </si>
+  <si>
     <t>Distrikt Beer</t>
   </si>
   <si>
@@ -603,6 +975,27 @@
     <t>https://www.openstreetmap.org/node/3512397640</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/distrikt-beer/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/distrikt-beer-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/DistriktCraftBeer</t>
+  </si>
+  <si>
+    <t>https://twitter.com/distriktbeer</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/distrikt-beer.png</t>
+  </si>
+  <si>
+    <t>48.841814</t>
+  </si>
+  <si>
+    <t>1.949381</t>
+  </si>
+  <si>
     <t>La Baleine</t>
   </si>
   <si>
@@ -621,6 +1014,24 @@
     <t>https://www.openstreetmap.org/node/3515250017</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/la-baleine/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/la-baleine-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/labaleinebrasserie</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/la-baleine.png</t>
+  </si>
+  <si>
+    <t>48.862294</t>
+  </si>
+  <si>
+    <t>2.412696</t>
+  </si>
+  <si>
     <t>La Montreuilloise</t>
   </si>
   <si>
@@ -639,6 +1050,27 @@
     <t>https://www.openstreetmap.org/way/81845099</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/la-montreuilloise/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/la-montreuilloise-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/montreuilloise</t>
+  </si>
+  <si>
+    <t>https://twitter.com/BiereMontreuil</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/la-montreuilloise.png</t>
+  </si>
+  <si>
+    <t>48.86335</t>
+  </si>
+  <si>
+    <t>2.461255</t>
+  </si>
+  <si>
     <t>Les Brasseurs du Grand Paris</t>
   </si>
   <si>
@@ -657,19 +1089,46 @@
     <t>Levallois-Perret</t>
   </si>
   <si>
+    <t>06 70 29 54 98</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/3515331421</t>
   </si>
   <si>
-    <t>Outland</t>
-  </si>
-  <si>
-    <t>C’est à son retour de Californie que Yann se lance, en 2006, dans le brassage amateur. Trois ans plus tard, la brasserie Outland voit le jour à Bagnolet. Inspirées des styles de la côte Ouest des Etats-Unis, les bières Outland mettent à l’honneur les houblons de cette région et sont un hommage à ceux qui ont aidé à perfectionner techniques et recettes. En attendant l’installation prochaine d’une nouvelle brasserie, Outland brasse à la Brasserie Parisis... et enchaîne les collaborations !</t>
-  </si>
-  <si>
-    <t>After a trip to California in 2006, Yann decided to take up home brewing. Three years later, he opened Outland brewery in Bagnolet. Heavily inspired by the US west-coast style of beer, his distinctly hoppy beers are a salute to all those in the region who have helped perfect brewing techniques and recipes. While waiting for the new (bigger!) brewery to open, Outland brews at the Parisis brewery--and contines to brew one collaboration after another!</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/brasserieoutland</t>
+    <t>http://laparisbeerweek.com/2015/programme/participant/les-brasseurs-du-grand-paris/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/les-brasseurs-du-grand-paris-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/mybeer</t>
+  </si>
+  <si>
+    <t>https://twitter.com/BeerGrandParis</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/les-brasseurs-du-grand-paris.png</t>
+  </si>
+  <si>
+    <t>48.892792</t>
+  </si>
+  <si>
+    <t>2.291969</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/node/3515412159</t>
+  </si>
+  <si>
+    <t>Parisis</t>
+  </si>
+  <si>
+    <t>La brasserie Parisis naît en septembre 2012. Suite logique de la brasserie artisanale de l’Yvette, elle est la consécration de trois ans de travail initiés par Eric, rejoint dès 2011 par Jonathan, que suivront quelque temps plus tard Maxime, Samuel et Fabien. Leur objectif : faire de belles bières et contribuer au renouveau de la bière artisanale en Ile-de-France.</t>
+  </si>
+  <si>
+    <t>Parisis Brewery opened in September 2012. Originally the Yvette brewery, Parisis is the result of 3 years of hard work initiated by Eric, who was joined by Jonathan in 2011, and later by Maxime, Samuel and Fabien. Their goal: to make great beers and contribute to the rebirth of the craft beer movement in the greater Paris region.</t>
+  </si>
+  <si>
+    <t>http://brasserie-parisis.com/</t>
   </si>
   <si>
     <t>Bâtiment K</t>
@@ -681,19 +1140,22 @@
     <t>Epinay sous Sénart</t>
   </si>
   <si>
-    <t>https://www.openstreetmap.org/node/3515412159</t>
-  </si>
-  <si>
-    <t>Parisis</t>
-  </si>
-  <si>
-    <t>La brasserie Parisis naît en septembre 2012. Suite logique de la brasserie artisanale de l’Yvette, elle est la consécration de trois ans de travail initiés par Eric, rejoint dès 2011 par Jonathan, que suivront quelque temps plus tard Maxime, Samuel et Fabien. Leur objectif : faire de belles bières et contribuer au renouveau de la bière artisanale en Ile-de-France.</t>
-  </si>
-  <si>
-    <t>Parisis Brewery opened in September 2012. Originally the Yvette brewery, Parisis is the result of 3 years of hard work initiated by Eric, who was joined by Jonathan in 2011, and later by Maxime, Samuel and Fabien. Their goal: to make great beers and contribute to the rebirth of the craft beer movement in the greater Paris region.</t>
-  </si>
-  <si>
-    <t>http://brasserie-parisis.com/</t>
+    <t>http://laparisbeerweek.com/2015/programme/participant/parisis/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/parisis-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/brasserieparisis</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/parisis.png</t>
+  </si>
+  <si>
+    <t>48.688744</t>
+  </si>
+  <si>
+    <t>2.513039</t>
   </si>
   <si>
     <t>DBI</t>
@@ -714,9 +1176,27 @@
     <t>du Dr Heulin</t>
   </si>
   <si>
+    <t>06 99 70 06 73</t>
+  </si>
+  <si>
     <t>https://www.openstreetmap.org/node/3515659468</t>
   </si>
   <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/dbi/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/dbi-en/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/dbi.png</t>
+  </si>
+  <si>
+    <t>48.890419</t>
+  </si>
+  <si>
+    <t>2.323739</t>
+  </si>
+  <si>
     <t>Enolia - 32 Via dei Birrai</t>
   </si>
   <si>
@@ -733,13 +1213,34 @@
   </si>
   <si>
     <t>https://www.openstreetmap.org/node/3515664840</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/enolia-32-via-dei-birrai/</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/programme/participant/enolia-32-via-dei-birrai-en/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/32viadeibirrai</t>
+  </si>
+  <si>
+    <t>https://twitter.com/32Viadeibirrai</t>
+  </si>
+  <si>
+    <t>http://laparisbeerweek.com/2015/visuels-participants/enolia-32-via-dei-birrai.png</t>
+  </si>
+  <si>
+    <t>48.873043</t>
+  </si>
+  <si>
+    <t>2.342355</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -767,19 +1268,6 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -801,7 +1289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -809,8 +1297,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1091,22 +1581,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="30.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
@@ -1117,14 +1607,16 @@
     <col min="12" max="12" width="20.42578125" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" customWidth="1"/>
     <col min="14" max="14" width="47.42578125" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" customWidth="1"/>
     <col min="16" max="16" width="38" customWidth="1"/>
     <col min="17" max="18" width="11.42578125" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" customWidth="1"/>
     <col min="20" max="21" width="56.140625" customWidth="1"/>
     <col min="22" max="22" width="15.28515625" customWidth="1"/>
-    <col min="23" max="23" width="8.7109375" customWidth="1"/>
-    <col min="24" max="26" width="14.42578125" customWidth="1"/>
+    <col min="23" max="23" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" customWidth="1"/>
+    <col min="26" max="26" width="47.140625" customWidth="1"/>
     <col min="27" max="28" width="8.7109375" customWidth="1"/>
     <col min="29" max="29" width="11.42578125" customWidth="1"/>
   </cols>
@@ -1257,17 +1749,17 @@
         <v>37</v>
       </c>
       <c r="N2" s="1" t="str">
-        <f t="shared" ref="N2:N27" si="0">CONCATENATE(G2,", ",I2," ",J2,", ",K2," ",L2,", ",M2)</f>
+        <f t="shared" ref="N2:N10" si="0">CONCATENATE(G2,", ",I2," ",J2,", ",K2," ",L2,", ",M2)</f>
         <v>62, RUE Quincampoix, 75004 Paris, FRANCE</v>
       </c>
-      <c r="O2" s="4">
-        <v>1</v>
-      </c>
-      <c r="P2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>39</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="R2" s="5">
         <v>1</v>
@@ -1275,26 +1767,32 @@
       <c r="S2" s="5">
         <v>1</v>
       </c>
-      <c r="T2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="8" t="s">
+      <c r="T2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="U2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="V2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="W2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="X2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="Y2" s="9" t="s">
         <v>46</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:29">
@@ -1302,19 +1800,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
@@ -1324,7 +1822,7 @@
         <v>34</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="K3" s="4">
         <v>75012</v>
@@ -1339,57 +1837,71 @@
         <f t="shared" si="0"/>
         <v>1, RUE de Lyon, 75012 Paris, FRANCE</v>
       </c>
-      <c r="O3" s="4">
-        <v>1</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
+      <c r="O3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
       <c r="S3" s="5">
         <v>1</v>
       </c>
-      <c r="T3" s="9"/>
-      <c r="U3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="G4" s="4">
         <v>4</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="K4" s="4">
         <v>75011</v>
@@ -1404,45 +1916,59 @@
         <f t="shared" si="0"/>
         <v>4, AVENUE Jean Aicard, 75011 Paris, FRANCE</v>
       </c>
-      <c r="O4" s="4">
-        <v>1</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
+      <c r="O4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
       <c r="S4" s="5">
         <v>1</v>
       </c>
-      <c r="T4" s="9"/>
-      <c r="U4" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="W4" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="X4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA4" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB4" s="10" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="G5" s="4">
         <v>10</v>
@@ -1452,7 +1978,7 @@
         <v>34</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="K5" s="4">
         <v>75018</v>
@@ -1467,45 +1993,57 @@
         <f t="shared" si="0"/>
         <v>10, RUE de la Fontaine du But, 75018 Paris, FRANCE</v>
       </c>
-      <c r="O5" s="4">
-        <v>1</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
       <c r="S5" s="5">
         <v>1</v>
       </c>
-      <c r="T5" s="9"/>
-      <c r="U5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="X5" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB5" s="10" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="G6" s="4">
         <v>3</v>
@@ -1515,7 +2053,7 @@
         <v>34</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="K6" s="4">
         <v>75018</v>
@@ -1530,45 +2068,59 @@
         <f t="shared" si="0"/>
         <v>3, RUE Baudelique, 75018 Paris, FRANCE</v>
       </c>
-      <c r="O6" s="4">
-        <v>1</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
+      <c r="O6" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
       <c r="S6" s="5">
         <v>1</v>
       </c>
-      <c r="T6" s="9"/>
-      <c r="U6" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X6" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA6" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB6" s="10" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="G7" s="4">
         <v>11</v>
@@ -1578,7 +2130,7 @@
         <v>34</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="K7" s="4">
         <v>75020</v>
@@ -1593,45 +2145,59 @@
         <f t="shared" si="0"/>
         <v>11, RUE Victor Letalle, 75020 Paris, FRANCE</v>
       </c>
-      <c r="O7" s="4">
-        <v>1</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
+      <c r="O7" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
       <c r="S7" s="5">
         <v>1</v>
       </c>
-      <c r="T7" s="9"/>
-      <c r="U7" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="V7" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="W7" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="X7" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA7" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB7" s="10" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="G8" s="4">
         <v>353</v>
@@ -1641,7 +2207,7 @@
         <v>34</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>89</v>
+        <v>126</v>
       </c>
       <c r="K8" s="4">
         <v>75020</v>
@@ -1656,56 +2222,70 @@
         <f t="shared" si="0"/>
         <v>353, RUE des Pyrénées, 75020 Paris, FRANCE</v>
       </c>
-      <c r="O8" s="4">
-        <v>1</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
       <c r="S8" s="5">
         <v>1</v>
       </c>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="V8" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA8" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB8" s="10" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="9" spans="1:29">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="G9" s="4">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="K9" s="4">
-        <v>75005</v>
+        <v>75018</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>36</v>
@@ -1715,60 +2295,72 @@
       </c>
       <c r="N9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>44, RUE des Boulangers, 75005 Paris, FRANCE</v>
-      </c>
-      <c r="O9" s="4">
-        <v>1</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
+        <v>20, RUE Custine, 75018 Paris, FRANCE</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
       <c r="S9" s="5">
         <v>1</v>
       </c>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="9"/>
-      <c r="Z9" s="9"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="V9" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="W9" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="X9" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA9" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB9" s="10" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="10" spans="1:29">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="G10" s="4">
-        <v>85</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="K10" s="4">
-        <v>75010</v>
+        <v>75005</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>36</v>
@@ -1778,57 +2370,72 @@
       </c>
       <c r="N10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>85, BOULEVARD de Magenta, 75010 Paris, FRANCE</v>
-      </c>
-      <c r="O10" s="4">
-        <v>1</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
+        <v>44, RUE des Boulangers, 75005 Paris, FRANCE</v>
+      </c>
+      <c r="O10" s="7"/>
+      <c r="P10" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
       <c r="S10" s="5">
         <v>1</v>
       </c>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="V10" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="W10" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="X10" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA10" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB10" s="10" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="11" spans="1:29">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>104</v>
+        <v>153</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="G11" s="4">
-        <v>32</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>108</v>
+        <v>154</v>
       </c>
       <c r="K11" s="4">
-        <v>75013</v>
+        <v>75018</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>36</v>
@@ -1836,62 +2443,73 @@
       <c r="M11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>32, RUE de l'Espérance, 75013 Paris, FRANCE</v>
-      </c>
-      <c r="O11" s="4">
-        <v>1</v>
-      </c>
-      <c r="P11" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
+      <c r="N11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
       <c r="S11" s="5">
         <v>1</v>
       </c>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="V11" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="W11" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="X11" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA11" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB11" s="10" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="G12" s="4">
-        <v>18</v>
-      </c>
-      <c r="H12" s="4">
-        <v>11</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="K12" s="4">
-        <v>75005</v>
+        <v>75017</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>36</v>
@@ -1899,59 +2517,73 @@
       <c r="M12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>18, RUE du Pot-de-Fer, 75005 Paris, FRANCE</v>
-      </c>
-      <c r="O12" s="4">
-        <v>1</v>
-      </c>
-      <c r="P12" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
+      <c r="N12" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
       <c r="S12" s="5">
         <v>1</v>
       </c>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="V12" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="W12" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="X12" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA12" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB12" s="10" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="G13" s="4">
-        <v>45</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H13" s="4"/>
       <c r="I13" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="K13" s="4">
-        <v>75014</v>
+        <v>75001</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>36</v>
@@ -1959,59 +2591,75 @@
       <c r="M13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>45, RUE de Gergovie, 75014 Paris, FRANCE</v>
-      </c>
-      <c r="O13" s="4">
-        <v>1</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
+      <c r="N13" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
       <c r="S13" s="5">
         <v>1</v>
       </c>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="X13" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA13" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="AB13" s="10" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G14" s="4">
         <v>85</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="G14" s="4">
-        <v>45</v>
+      <c r="H14" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>34</v>
+        <v>175</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>35</v>
+        <v>176</v>
       </c>
       <c r="K14" s="4">
-        <v>75004</v>
+        <v>75010</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>36</v>
@@ -2020,119 +2668,151 @@
         <v>37</v>
       </c>
       <c r="N14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>45, RUE Quincampoix, 75004 Paris, FRANCE</v>
-      </c>
-      <c r="O14" s="4">
-        <v>1</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
+        <f t="shared" ref="N14:N30" si="1">CONCATENATE(G14,", ",I14," ",J14,", ",K14," ",L14,", ",M14)</f>
+        <v>85, BOULEVARD de Magenta, 75010 Paris, FRANCE</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
       <c r="S14" s="5">
         <v>1</v>
       </c>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="V14" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="W14" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA14" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB14" s="10" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>127</v>
+        <v>185</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>131</v>
+        <v>188</v>
       </c>
       <c r="G15" s="4">
-        <v>50</v>
-      </c>
-      <c r="H15" s="4"/>
+        <v>32</v>
+      </c>
       <c r="I15" s="4" t="s">
-        <v>132</v>
+        <v>34</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>133</v>
+        <v>189</v>
       </c>
       <c r="K15" s="4">
-        <v>91460</v>
+        <v>75013</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>134</v>
+        <v>36</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="N15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>50, ROUTE d'Orsay, 91460 Marcoussis, FRANCE</v>
-      </c>
-      <c r="O15" s="4">
-        <v>1</v>
-      </c>
-      <c r="P15" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
+        <f t="shared" si="1"/>
+        <v>32, RUE de l'Espérance, 75013 Paris, FRANCE</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
       <c r="S15" s="5">
         <v>1</v>
       </c>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="9"/>
-      <c r="Z15" s="9"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="V15" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="W15" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="X15" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA15" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB15" s="10" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>136</v>
+        <v>199</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>137</v>
+        <v>200</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>138</v>
+        <v>201</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>139</v>
+        <v>202</v>
       </c>
       <c r="G16" s="4">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="H16" s="4">
+        <v>11</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>140</v>
+        <v>203</v>
       </c>
       <c r="K16" s="4">
-        <v>75018</v>
+        <v>75005</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>36</v>
@@ -2141,699 +2821,1085 @@
         <v>37</v>
       </c>
       <c r="N16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>28, RUE de la Goutte d'Or, 75018 Paris, FRANCE</v>
-      </c>
-      <c r="O16" s="4">
-        <v>1</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
+        <f t="shared" si="1"/>
+        <v>18, RUE du Pot-de-Fer, 75005 Paris, FRANCE</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
       <c r="S16" s="5">
         <v>1</v>
       </c>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16" s="9"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="V16" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="W16" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA16" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="AB16" s="10" t="s">
+        <v>211</v>
+      </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:28">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>142</v>
+        <v>212</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>143</v>
+        <v>213</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>144</v>
+        <v>214</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>145</v>
+        <v>215</v>
       </c>
       <c r="G17" s="4">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>146</v>
+        <v>216</v>
       </c>
       <c r="K17" s="4">
-        <v>78830</v>
+        <v>75014</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>147</v>
+        <v>36</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>37</v>
       </c>
       <c r="N17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>65, RUE de la Division Leclerc, 78830 Bonnelles, FRANCE</v>
-      </c>
-      <c r="O17" s="4">
-        <v>1</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
+        <f t="shared" si="1"/>
+        <v>45, RUE de Gergovie, 75014 Paris, FRANCE</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
       <c r="S17" s="5">
         <v>1</v>
       </c>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="9"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="V17" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="X17" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA17" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="AB17" s="10" t="s">
+        <v>225</v>
+      </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:28">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>149</v>
+        <v>226</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>150</v>
+        <v>227</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>151</v>
+        <v>228</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>153</v>
+        <v>229</v>
+      </c>
+      <c r="G18" s="4">
+        <v>45</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>154</v>
+        <v>35</v>
       </c>
       <c r="K18" s="4">
-        <v>77710</v>
+        <v>75004</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>155</v>
+        <v>36</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="N18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>, RUE de La tuilerie, 77710 Vaux-Sur-Lunain, FRANCE</v>
-      </c>
-      <c r="O18" s="4">
-        <v>1</v>
-      </c>
-      <c r="P18" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
+        <f t="shared" si="1"/>
+        <v>45, RUE Quincampoix, 75004 Paris, FRANCE</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
       <c r="S18" s="5">
         <v>1</v>
       </c>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="9"/>
-      <c r="Z18" s="9"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="V18" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="W18" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA18" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="AB18" s="10" t="s">
+        <v>237</v>
+      </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:28">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>157</v>
+        <v>238</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>128</v>
+        <v>239</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>158</v>
+        <v>240</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>159</v>
+        <v>241</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>160</v>
+        <v>242</v>
       </c>
       <c r="G19" s="4">
-        <v>71</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="H19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>34</v>
+        <v>243</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>161</v>
+        <v>244</v>
       </c>
       <c r="K19" s="4">
-        <v>93100</v>
+        <v>91460</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>162</v>
+        <v>245</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>37</v>
       </c>
       <c r="N19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>71, RUE de la Fraternité, 93100 Montreuil, FRANCE</v>
-      </c>
-      <c r="O19" s="4">
-        <v>1</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
+        <f t="shared" si="1"/>
+        <v>50, ROUTE d'Orsay, 91460 Marcoussis, FRANCE</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
       <c r="S19" s="5">
         <v>1</v>
       </c>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="V19" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="W19" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA19" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="AB19" s="10" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:28">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>164</v>
+        <v>254</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>128</v>
+        <v>239</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>166</v>
+        <v>256</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>167</v>
+        <v>257</v>
       </c>
       <c r="G20" s="4">
-        <v>50</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>168</v>
+        <v>28</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>132</v>
+        <v>34</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>169</v>
+        <v>258</v>
       </c>
       <c r="K20" s="4">
-        <v>78850</v>
+        <v>75018</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>170</v>
+        <v>36</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>37</v>
       </c>
       <c r="N20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>50, ROUTE de la Ferme, 78850 Thiverval-Grignon, FRANCE</v>
-      </c>
-      <c r="O20" s="4">
-        <v>1</v>
-      </c>
-      <c r="P20" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
+        <f t="shared" si="1"/>
+        <v>28, RUE de la Goutte d'Or, 75018 Paris, FRANCE</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
       <c r="S20" s="5">
         <v>1</v>
       </c>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="V20" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="W20" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="X20" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="AA20" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="AB20" s="10" t="s">
+        <v>267</v>
+      </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:28">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>172</v>
+        <v>268</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>128</v>
+        <v>239</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>173</v>
+        <v>269</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>174</v>
+        <v>270</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>175</v>
+        <v>271</v>
       </c>
       <c r="G21" s="4">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>176</v>
+        <v>272</v>
       </c>
       <c r="K21" s="4">
-        <v>75020</v>
+        <v>78830</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>36</v>
+        <v>273</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>37</v>
       </c>
       <c r="N21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>17, RUE Henri Duvernois, 75020 Paris, FRANCE</v>
-      </c>
-      <c r="O21" s="4">
-        <v>1</v>
-      </c>
-      <c r="P21" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
+        <f t="shared" si="1"/>
+        <v>65, RUE de la Division Leclerc, 78830 Bonnelles, FRANCE</v>
+      </c>
+      <c r="O21" s="7"/>
+      <c r="P21" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
       <c r="S21" s="5">
         <v>1</v>
       </c>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="V21" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA21" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="AB21" s="10" t="s">
+        <v>279</v>
+      </c>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:28">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>178</v>
+        <v>280</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>128</v>
+        <v>239</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>179</v>
+        <v>281</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>180</v>
+        <v>282</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="G22" s="4">
-        <v>97</v>
+        <v>283</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>284</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>182</v>
+        <v>285</v>
       </c>
       <c r="K22" s="4">
-        <v>93100</v>
+        <v>77710</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>162</v>
+        <v>286</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>37</v>
       </c>
       <c r="N22" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>97, RUE Pierre de Montreuil, 93100 Montreuil, FRANCE</v>
-      </c>
-      <c r="O22" s="4">
-        <v>1</v>
-      </c>
-      <c r="P22" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
+        <f t="shared" si="1"/>
+        <v>, RUE de La tuilerie, 77710 Vaux-Sur-Lunain, FRANCE</v>
+      </c>
+      <c r="O22" s="7"/>
+      <c r="P22" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
       <c r="S22" s="5">
         <v>1</v>
       </c>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="V22" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="W22" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="AA22" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="AB22" s="10" t="s">
+        <v>293</v>
+      </c>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:28">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>184</v>
+        <v>294</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>128</v>
+        <v>239</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>185</v>
+        <v>295</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>186</v>
+        <v>296</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>187</v>
+        <v>297</v>
       </c>
       <c r="G23" s="4">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>188</v>
+        <v>298</v>
       </c>
       <c r="K23" s="4">
-        <v>92300</v>
+        <v>93100</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>189</v>
+        <v>299</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="N23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>106, RUE Louis Rouquier, 92300 Levallois-Perret, FRANCE</v>
-      </c>
-      <c r="O23" s="4">
-        <v>1</v>
-      </c>
-      <c r="P23" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
+        <f t="shared" si="1"/>
+        <v>71, RUE de la Fraternité, 93100 Montreuil, FRANCE</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="P23" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
       <c r="S23" s="5">
         <v>1</v>
       </c>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="9"/>
-      <c r="Z23" s="9"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="W23" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="X23" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="AA23" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="AB23" s="10" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:28">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>191</v>
+        <v>309</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>128</v>
+        <v>239</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>192</v>
+        <v>310</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>193</v>
+        <v>311</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>194</v>
+        <v>312</v>
       </c>
       <c r="G24" s="4">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>195</v>
+        <v>313</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>34</v>
+        <v>243</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>196</v>
+        <v>314</v>
       </c>
       <c r="K24" s="4">
-        <v>91860</v>
+        <v>78850</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>197</v>
+        <v>315</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="N24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>34, RUE de la Forêt, 91860 Epinay sous Sénart, FRANCE</v>
-      </c>
-      <c r="O24" s="4">
-        <v>1</v>
-      </c>
-      <c r="P24" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
+        <f t="shared" si="1"/>
+        <v>50, ROUTE de la Ferme, 78850 Thiverval-Grignon, FRANCE</v>
+      </c>
+      <c r="O24" s="7"/>
+      <c r="P24" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
       <c r="S24" s="5">
         <v>1</v>
       </c>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
-      <c r="X24" s="9"/>
-      <c r="Y24" s="9"/>
-      <c r="Z24" s="9"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="V24" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="W24" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="X24" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="AA24" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB24" s="10" t="s">
+        <v>323</v>
+      </c>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:28">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>199</v>
+        <v>324</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>128</v>
+        <v>239</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>200</v>
+        <v>325</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>201</v>
+        <v>326</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>202</v>
+        <v>327</v>
       </c>
       <c r="G25" s="4">
-        <v>34</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>195</v>
+        <v>17</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>196</v>
+        <v>328</v>
       </c>
       <c r="K25" s="4">
-        <v>91860</v>
+        <v>75020</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>197</v>
+        <v>36</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>37</v>
       </c>
       <c r="N25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>34, RUE de la Forêt, 91860 Epinay sous Sénart, FRANCE</v>
-      </c>
-      <c r="O25" s="4">
-        <v>1</v>
-      </c>
-      <c r="P25" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
+        <f t="shared" si="1"/>
+        <v>17, RUE Henri Duvernois, 75020 Paris, FRANCE</v>
+      </c>
+      <c r="O25" s="7"/>
+      <c r="P25" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
       <c r="S25" s="5">
         <v>1</v>
       </c>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
-      <c r="W25" s="9"/>
-      <c r="X25" s="9"/>
-      <c r="Y25" s="9"/>
-      <c r="Z25" s="9"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="V25" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="W25" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="AA25" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="AB25" s="10" t="s">
+        <v>335</v>
+      </c>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:28">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>203</v>
+        <v>336</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>204</v>
+        <v>239</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>205</v>
+        <v>337</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>206</v>
+        <v>338</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>207</v>
+        <v>339</v>
       </c>
       <c r="G26" s="4">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>208</v>
+        <v>340</v>
       </c>
       <c r="K26" s="4">
-        <v>75017</v>
+        <v>93100</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>36</v>
+        <v>299</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>37</v>
       </c>
       <c r="N26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>27, RUE du Dr Heulin, 75017 Paris, FRANCE</v>
-      </c>
-      <c r="O26" s="4">
-        <v>1</v>
-      </c>
-      <c r="P26" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
+        <f t="shared" si="1"/>
+        <v>97, RUE Pierre de Montreuil, 93100 Montreuil, FRANCE</v>
+      </c>
+      <c r="O26" s="7"/>
+      <c r="P26" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
       <c r="S26" s="5">
         <v>1</v>
       </c>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
-      <c r="W26" s="9"/>
-      <c r="X26" s="9"/>
-      <c r="Y26" s="9"/>
-      <c r="Z26" s="9"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="V26" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="W26" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="X26" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="AA26" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="AB26" s="10" t="s">
+        <v>348</v>
+      </c>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:28">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>210</v>
+        <v>349</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>204</v>
+        <v>239</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>211</v>
+        <v>350</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>212</v>
+        <v>351</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>213</v>
+        <v>352</v>
       </c>
       <c r="G27" s="4">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>214</v>
+        <v>353</v>
       </c>
       <c r="K27" s="4">
-        <v>75009</v>
+        <v>92300</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>36</v>
+        <v>354</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>37</v>
       </c>
       <c r="N27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>6, RUE de la Grange Batelière, 75009 Paris, FRANCE</v>
-      </c>
-      <c r="O27" s="4">
-        <v>1</v>
-      </c>
-      <c r="P27" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
+        <f t="shared" si="1"/>
+        <v>106, RUE Louis Rouquier, 92300 Levallois-Perret, FRANCE</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="P27" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
       <c r="S27" s="5">
         <v>1</v>
       </c>
-      <c r="T27" s="9"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="9"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="V27" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="W27" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="X27" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="AA27" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="AB27" s="10" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28">
+      <c r="A28" s="3">
+        <v>28</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="G28" s="4">
+        <v>34</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="K28" s="4">
+        <v>91860</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34, RUE de la Forêt, 91860 Epinay sous Sénart, FRANCE</v>
+      </c>
+      <c r="O28" s="7"/>
+      <c r="P28" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="5">
+        <v>1</v>
+      </c>
+      <c r="T28" s="11"/>
+      <c r="U28" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="V28" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="W28" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="AA28" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="AB28" s="10" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28">
+      <c r="A29" s="3">
+        <v>29</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="G29" s="4">
+        <v>27</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="K29" s="4">
+        <v>75017</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>27, RUE du Dr Heulin, 75017 Paris, FRANCE</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="P29" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="5">
+        <v>1</v>
+      </c>
+      <c r="T29" s="11"/>
+      <c r="U29" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="V29" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="W29" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="X29" s="11"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="AA29" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="AB29" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28">
+      <c r="A30" s="3">
+        <v>30</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="G30" s="4">
+        <v>6</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="K30" s="4">
+        <v>75009</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>6, RUE de la Grange Batelière, 75009 Paris, FRANCE</v>
+      </c>
+      <c r="O30" s="7"/>
+      <c r="P30" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="5">
+        <v>1</v>
+      </c>
+      <c r="T30" s="11"/>
+      <c r="U30" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="V30" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="W30" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="X30" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA30" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="AB30" s="10" t="s">
+        <v>403</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC27"/>
+  <autoFilter ref="A1:AC30"/>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="P2" r:id="rId2"/>
@@ -2848,60 +3914,190 @@
     <hyperlink ref="F3" r:id="rId11"/>
     <hyperlink ref="P3" r:id="rId12"/>
     <hyperlink ref="U3" r:id="rId13"/>
-    <hyperlink ref="F4" r:id="rId14"/>
-    <hyperlink ref="P4" r:id="rId15"/>
-    <hyperlink ref="U4" r:id="rId16"/>
-    <hyperlink ref="F5" r:id="rId17"/>
-    <hyperlink ref="P5" r:id="rId18"/>
-    <hyperlink ref="U5" r:id="rId19"/>
-    <hyperlink ref="F6" r:id="rId20"/>
-    <hyperlink ref="P6" r:id="rId21"/>
-    <hyperlink ref="U6" r:id="rId22"/>
-    <hyperlink ref="F7" r:id="rId23"/>
-    <hyperlink ref="P7" r:id="rId24"/>
-    <hyperlink ref="U7" r:id="rId25"/>
-    <hyperlink ref="F8" r:id="rId26"/>
-    <hyperlink ref="P8" r:id="rId27"/>
-    <hyperlink ref="F9" r:id="rId28"/>
-    <hyperlink ref="P9" r:id="rId29"/>
-    <hyperlink ref="F10" r:id="rId30"/>
-    <hyperlink ref="P10" r:id="rId31"/>
-    <hyperlink ref="F11" r:id="rId32"/>
-    <hyperlink ref="P11" r:id="rId33"/>
-    <hyperlink ref="F12" r:id="rId34"/>
-    <hyperlink ref="P12" r:id="rId35"/>
-    <hyperlink ref="F13" r:id="rId36"/>
-    <hyperlink ref="P13" r:id="rId37"/>
-    <hyperlink ref="F14" r:id="rId38"/>
-    <hyperlink ref="P14" r:id="rId39"/>
-    <hyperlink ref="F15" r:id="rId40"/>
-    <hyperlink ref="P15" r:id="rId41"/>
-    <hyperlink ref="F16" r:id="rId42"/>
-    <hyperlink ref="P16" r:id="rId43"/>
-    <hyperlink ref="F17" r:id="rId44"/>
-    <hyperlink ref="P17" r:id="rId45"/>
-    <hyperlink ref="F18" r:id="rId46"/>
-    <hyperlink ref="P18" r:id="rId47"/>
-    <hyperlink ref="F19" r:id="rId48"/>
-    <hyperlink ref="P19" r:id="rId49"/>
-    <hyperlink ref="F20" r:id="rId50"/>
-    <hyperlink ref="P20" r:id="rId51"/>
-    <hyperlink ref="F21" r:id="rId52"/>
-    <hyperlink ref="P21" r:id="rId53"/>
-    <hyperlink ref="F22" r:id="rId54"/>
-    <hyperlink ref="P22" r:id="rId55"/>
-    <hyperlink ref="F23" r:id="rId56"/>
-    <hyperlink ref="P23" r:id="rId57"/>
-    <hyperlink ref="F24" r:id="rId58"/>
-    <hyperlink ref="P24" r:id="rId59"/>
-    <hyperlink ref="F25" r:id="rId60"/>
-    <hyperlink ref="P25" r:id="rId61"/>
-    <hyperlink ref="F26" r:id="rId62"/>
-    <hyperlink ref="P26" r:id="rId63"/>
-    <hyperlink ref="F27" r:id="rId64"/>
-    <hyperlink ref="P27" r:id="rId65"/>
+    <hyperlink ref="V3" r:id="rId14"/>
+    <hyperlink ref="W3" r:id="rId15"/>
+    <hyperlink ref="X3" r:id="rId16"/>
+    <hyperlink ref="Z3" r:id="rId17"/>
+    <hyperlink ref="F4" r:id="rId18"/>
+    <hyperlink ref="P4" r:id="rId19"/>
+    <hyperlink ref="U4" r:id="rId20"/>
+    <hyperlink ref="V4" r:id="rId21"/>
+    <hyperlink ref="W4" r:id="rId22"/>
+    <hyperlink ref="X4" r:id="rId23"/>
+    <hyperlink ref="Z4" r:id="rId24"/>
+    <hyperlink ref="F5" r:id="rId25"/>
+    <hyperlink ref="P5" r:id="rId26"/>
+    <hyperlink ref="U5" r:id="rId27"/>
+    <hyperlink ref="V5" r:id="rId28"/>
+    <hyperlink ref="W5" r:id="rId29"/>
+    <hyperlink ref="X5" r:id="rId30"/>
+    <hyperlink ref="Z5" r:id="rId31"/>
+    <hyperlink ref="F6" r:id="rId32"/>
+    <hyperlink ref="P6" r:id="rId33"/>
+    <hyperlink ref="U6" r:id="rId34"/>
+    <hyperlink ref="V6" r:id="rId35"/>
+    <hyperlink ref="W6" r:id="rId36"/>
+    <hyperlink ref="X6" r:id="rId37"/>
+    <hyperlink ref="Z6" r:id="rId38"/>
+    <hyperlink ref="F7" r:id="rId39"/>
+    <hyperlink ref="P7" r:id="rId40"/>
+    <hyperlink ref="U7" r:id="rId41"/>
+    <hyperlink ref="V7" r:id="rId42"/>
+    <hyperlink ref="W7" r:id="rId43"/>
+    <hyperlink ref="X7" r:id="rId44"/>
+    <hyperlink ref="Z7" r:id="rId45"/>
+    <hyperlink ref="F8" r:id="rId46"/>
+    <hyperlink ref="P8" r:id="rId47"/>
+    <hyperlink ref="U8" r:id="rId48"/>
+    <hyperlink ref="V8" r:id="rId49"/>
+    <hyperlink ref="W8" r:id="rId50"/>
+    <hyperlink ref="X8" r:id="rId51"/>
+    <hyperlink ref="Z8" r:id="rId52"/>
+    <hyperlink ref="F9" r:id="rId53"/>
+    <hyperlink ref="P9" r:id="rId54"/>
+    <hyperlink ref="U9" r:id="rId55"/>
+    <hyperlink ref="V9" r:id="rId56"/>
+    <hyperlink ref="W9" r:id="rId57"/>
+    <hyperlink ref="X9" r:id="rId58"/>
+    <hyperlink ref="Z9" r:id="rId59"/>
+    <hyperlink ref="F10" r:id="rId60"/>
+    <hyperlink ref="P10" r:id="rId61"/>
+    <hyperlink ref="U10" r:id="rId62"/>
+    <hyperlink ref="V10" r:id="rId63"/>
+    <hyperlink ref="W10" r:id="rId64"/>
+    <hyperlink ref="X10" r:id="rId65"/>
+    <hyperlink ref="Z10" r:id="rId66"/>
+    <hyperlink ref="F11" r:id="rId67"/>
+    <hyperlink ref="P11" r:id="rId68" location="map=19/48.88955/2.33380"/>
+    <hyperlink ref="U11" r:id="rId69"/>
+    <hyperlink ref="V11" r:id="rId70"/>
+    <hyperlink ref="W11" r:id="rId71"/>
+    <hyperlink ref="X11" r:id="rId72"/>
+    <hyperlink ref="Z11" r:id="rId73"/>
+    <hyperlink ref="F12" r:id="rId74"/>
+    <hyperlink ref="P12" r:id="rId75"/>
+    <hyperlink ref="U12" r:id="rId76"/>
+    <hyperlink ref="V12" r:id="rId77"/>
+    <hyperlink ref="W12" r:id="rId78"/>
+    <hyperlink ref="X12" r:id="rId79"/>
+    <hyperlink ref="Z12" r:id="rId80"/>
+    <hyperlink ref="F13" r:id="rId81"/>
+    <hyperlink ref="P13" r:id="rId82" location="map=19/48.85986/2.34681"/>
+    <hyperlink ref="U13" r:id="rId83"/>
+    <hyperlink ref="V13" r:id="rId84"/>
+    <hyperlink ref="W13" r:id="rId85"/>
+    <hyperlink ref="X13" r:id="rId86"/>
+    <hyperlink ref="Z13" r:id="rId87"/>
+    <hyperlink ref="F14" r:id="rId88"/>
+    <hyperlink ref="P14" r:id="rId89"/>
+    <hyperlink ref="U14" r:id="rId90"/>
+    <hyperlink ref="V14" r:id="rId91"/>
+    <hyperlink ref="W14" r:id="rId92"/>
+    <hyperlink ref="Z14" r:id="rId93"/>
+    <hyperlink ref="F15" r:id="rId94"/>
+    <hyperlink ref="P15" r:id="rId95"/>
+    <hyperlink ref="U15" r:id="rId96"/>
+    <hyperlink ref="V15" r:id="rId97"/>
+    <hyperlink ref="W15" r:id="rId98"/>
+    <hyperlink ref="X15" r:id="rId99"/>
+    <hyperlink ref="Z15" r:id="rId100"/>
+    <hyperlink ref="F16" r:id="rId101"/>
+    <hyperlink ref="P16" r:id="rId102"/>
+    <hyperlink ref="U16" r:id="rId103"/>
+    <hyperlink ref="V16" r:id="rId104"/>
+    <hyperlink ref="W16" r:id="rId105"/>
+    <hyperlink ref="Z16" r:id="rId106"/>
+    <hyperlink ref="F17" r:id="rId107"/>
+    <hyperlink ref="P17" r:id="rId108"/>
+    <hyperlink ref="U17" r:id="rId109"/>
+    <hyperlink ref="V17" r:id="rId110"/>
+    <hyperlink ref="W17" r:id="rId111"/>
+    <hyperlink ref="X17" r:id="rId112"/>
+    <hyperlink ref="Z17" r:id="rId113"/>
+    <hyperlink ref="F18" r:id="rId114"/>
+    <hyperlink ref="P18" r:id="rId115"/>
+    <hyperlink ref="U18" r:id="rId116"/>
+    <hyperlink ref="V18" r:id="rId117"/>
+    <hyperlink ref="W18" r:id="rId118"/>
+    <hyperlink ref="Z18" r:id="rId119"/>
+    <hyperlink ref="F19" r:id="rId120"/>
+    <hyperlink ref="P19" r:id="rId121"/>
+    <hyperlink ref="U19" r:id="rId122"/>
+    <hyperlink ref="V19" r:id="rId123"/>
+    <hyperlink ref="W19" r:id="rId124"/>
+    <hyperlink ref="Z19" r:id="rId125"/>
+    <hyperlink ref="F20" r:id="rId126"/>
+    <hyperlink ref="P20" r:id="rId127"/>
+    <hyperlink ref="U20" r:id="rId128"/>
+    <hyperlink ref="V20" r:id="rId129"/>
+    <hyperlink ref="W20" r:id="rId130"/>
+    <hyperlink ref="X20" r:id="rId131"/>
+    <hyperlink ref="Z20" r:id="rId132"/>
+    <hyperlink ref="F21" r:id="rId133"/>
+    <hyperlink ref="P21" r:id="rId134"/>
+    <hyperlink ref="U21" r:id="rId135"/>
+    <hyperlink ref="V21" r:id="rId136"/>
+    <hyperlink ref="Z21" r:id="rId137"/>
+    <hyperlink ref="F22" r:id="rId138"/>
+    <hyperlink ref="P22" r:id="rId139"/>
+    <hyperlink ref="U22" r:id="rId140"/>
+    <hyperlink ref="V22" r:id="rId141"/>
+    <hyperlink ref="W22" r:id="rId142"/>
+    <hyperlink ref="Z22" r:id="rId143"/>
+    <hyperlink ref="F23" r:id="rId144"/>
+    <hyperlink ref="P23" r:id="rId145"/>
+    <hyperlink ref="U23" r:id="rId146"/>
+    <hyperlink ref="V23" r:id="rId147"/>
+    <hyperlink ref="W23" r:id="rId148"/>
+    <hyperlink ref="X23" r:id="rId149"/>
+    <hyperlink ref="Z23" r:id="rId150"/>
+    <hyperlink ref="F24" r:id="rId151"/>
+    <hyperlink ref="P24" r:id="rId152"/>
+    <hyperlink ref="U24" r:id="rId153"/>
+    <hyperlink ref="V24" r:id="rId154"/>
+    <hyperlink ref="W24" r:id="rId155"/>
+    <hyperlink ref="X24" r:id="rId156"/>
+    <hyperlink ref="Z24" r:id="rId157"/>
+    <hyperlink ref="F25" r:id="rId158"/>
+    <hyperlink ref="P25" r:id="rId159"/>
+    <hyperlink ref="U25" r:id="rId160"/>
+    <hyperlink ref="V25" r:id="rId161"/>
+    <hyperlink ref="W25" r:id="rId162"/>
+    <hyperlink ref="Z25" r:id="rId163"/>
+    <hyperlink ref="F26" r:id="rId164"/>
+    <hyperlink ref="P26" r:id="rId165"/>
+    <hyperlink ref="U26" r:id="rId166"/>
+    <hyperlink ref="V26" r:id="rId167"/>
+    <hyperlink ref="W26" r:id="rId168"/>
+    <hyperlink ref="X26" r:id="rId169"/>
+    <hyperlink ref="Z26" r:id="rId170"/>
+    <hyperlink ref="F27" r:id="rId171"/>
+    <hyperlink ref="P27" r:id="rId172"/>
+    <hyperlink ref="U27" r:id="rId173"/>
+    <hyperlink ref="V27" r:id="rId174"/>
+    <hyperlink ref="W27" r:id="rId175"/>
+    <hyperlink ref="X27" r:id="rId176"/>
+    <hyperlink ref="Z27" r:id="rId177"/>
+    <hyperlink ref="F28" r:id="rId178"/>
+    <hyperlink ref="P28" r:id="rId179"/>
+    <hyperlink ref="U28" r:id="rId180"/>
+    <hyperlink ref="V28" r:id="rId181"/>
+    <hyperlink ref="W28" r:id="rId182"/>
+    <hyperlink ref="Z28" r:id="rId183"/>
+    <hyperlink ref="F29" r:id="rId184"/>
+    <hyperlink ref="P29" r:id="rId185"/>
+    <hyperlink ref="U29" r:id="rId186"/>
+    <hyperlink ref="V29" r:id="rId187"/>
+    <hyperlink ref="W29" r:id="rId188"/>
+    <hyperlink ref="Z29" r:id="rId189"/>
+    <hyperlink ref="F30" r:id="rId190"/>
+    <hyperlink ref="P30" r:id="rId191"/>
+    <hyperlink ref="U30" r:id="rId192"/>
+    <hyperlink ref="V30" r:id="rId193"/>
+    <hyperlink ref="W30" r:id="rId194"/>
+    <hyperlink ref="X30" r:id="rId195"/>
+    <hyperlink ref="Z30" r:id="rId196"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId66"/>
 </worksheet>
 </file>
</xml_diff>